<commit_message>
Updated test data in RTM
</commit_message>
<xml_diff>
--- a/Planetarium RTM.xlsx
+++ b/Planetarium RTM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="250">
   <si>
     <t>ID</t>
   </si>
@@ -728,7 +728,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>the user should not see the logout button</t>
+      <t>the user should stay on the login page</t>
     </r>
   </si>
   <si>
@@ -1796,7 +1796,7 @@
     <t>IPN1</t>
   </si>
   <si>
-    <t>NoPlanet</t>
+    <t>NotPlanet</t>
   </si>
   <si>
     <t>invalid username</t>
@@ -1868,10 +1868,10 @@
     <t>IMN3</t>
   </si>
   <si>
-    <t>invalid moon name alert</t>
-  </si>
-  <si>
-    <t>invalid planet name alert</t>
+    <t>Invalid moon name</t>
+  </si>
+  <si>
+    <t>Invalid planet name</t>
   </si>
   <si>
     <t>IU4</t>
@@ -1904,7 +1904,7 @@
     <t>invalid planet ID</t>
   </si>
   <si>
-    <t>login success</t>
+    <t>login success, redirect to home</t>
   </si>
   <si>
     <t>IFPT1</t>
@@ -1919,7 +1919,7 @@
     <t>IPID1</t>
   </si>
   <si>
-    <t>Invalid Credentials alert</t>
+    <t>Invalid Credentials</t>
   </si>
   <si>
     <t>IP2</t>
@@ -1958,9 +1958,6 @@
     <t>User State</t>
   </si>
   <si>
-    <t>Invalid planet name alert</t>
-  </si>
-  <si>
     <t>IP5</t>
   </si>
   <si>
@@ -1988,19 +1985,19 @@
     <t>IP7</t>
   </si>
   <si>
-    <t>Invalid file type alert</t>
-  </si>
-  <si>
-    <t>invalid planet ID alert</t>
-  </si>
-  <si>
-    <t>Account create successfully alert</t>
-  </si>
-  <si>
-    <t>Invalid username alert</t>
-  </si>
-  <si>
-    <t>Invalid password alert</t>
+    <t>Invalid file type</t>
+  </si>
+  <si>
+    <t>Invalid planet ID</t>
+  </si>
+  <si>
+    <t>Account created successfully</t>
+  </si>
+  <si>
+    <t>Invalid username</t>
+  </si>
+  <si>
+    <t>Invalid password</t>
   </si>
   <si>
     <t>User Requirement</t>
@@ -2279,7 +2276,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2477,6 +2474,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8548,7 +8548,7 @@
       <c r="E14" s="51" t="s">
         <v>147</v>
       </c>
-      <c r="F14" s="51" t="s">
+      <c r="F14" s="57" t="s">
         <v>196</v>
       </c>
       <c r="G14" s="52" t="s">
@@ -8592,7 +8592,7 @@
       <c r="E15" s="51" t="s">
         <v>179</v>
       </c>
-      <c r="F15" s="51" t="s">
+      <c r="F15" s="57" t="s">
         <v>201</v>
       </c>
       <c r="G15" s="60" t="s">
@@ -8626,7 +8626,7 @@
       <c r="E16" s="51" t="s">
         <v>147</v>
       </c>
-      <c r="F16" s="51" t="s">
+      <c r="F16" s="57" t="s">
         <v>201</v>
       </c>
       <c r="G16" s="64" t="s">
@@ -8670,7 +8670,7 @@
       <c r="E17" s="51" t="s">
         <v>179</v>
       </c>
-      <c r="F17" s="51" t="s">
+      <c r="F17" s="57" t="s">
         <v>201</v>
       </c>
       <c r="G17" s="52" t="s">
@@ -8721,7 +8721,7 @@
         <v>150</v>
       </c>
       <c r="I18" s="59" t="s">
-        <v>214</v>
+        <v>185</v>
       </c>
       <c r="J18" s="54" t="s">
         <v>156</v>
@@ -8741,19 +8741,19 @@
     </row>
     <row r="19">
       <c r="A19" s="51" t="s">
+        <v>214</v>
+      </c>
+      <c r="B19" s="51" t="s">
         <v>215</v>
-      </c>
-      <c r="B19" s="51" t="s">
-        <v>216</v>
       </c>
       <c r="C19" s="62" t="s">
         <v>18</v>
       </c>
       <c r="D19" s="51" t="s">
+        <v>216</v>
+      </c>
+      <c r="E19" s="51" t="s">
         <v>217</v>
-      </c>
-      <c r="E19" s="51" t="s">
-        <v>218</v>
       </c>
       <c r="G19" s="52" t="s">
         <v>171</v>
@@ -8762,7 +8762,7 @@
         <v>150</v>
       </c>
       <c r="I19" s="59" t="s">
-        <v>214</v>
+        <v>185</v>
       </c>
       <c r="J19" s="54" t="s">
         <v>173</v>
@@ -8782,19 +8782,19 @@
     </row>
     <row r="20">
       <c r="A20" s="51" t="s">
+        <v>218</v>
+      </c>
+      <c r="B20" s="51" t="s">
         <v>219</v>
-      </c>
-      <c r="B20" s="51" t="s">
-        <v>220</v>
       </c>
       <c r="C20" s="62" t="s">
         <v>18</v>
       </c>
       <c r="D20" s="51" t="s">
+        <v>220</v>
+      </c>
+      <c r="E20" s="51" t="s">
         <v>221</v>
-      </c>
-      <c r="E20" s="51" t="s">
-        <v>222</v>
       </c>
       <c r="G20" s="52" t="s">
         <v>181</v>
@@ -8803,7 +8803,7 @@
         <v>150</v>
       </c>
       <c r="I20" s="59" t="s">
-        <v>214</v>
+        <v>185</v>
       </c>
       <c r="J20" s="54" t="s">
         <v>183</v>
@@ -8823,7 +8823,7 @@
     </row>
     <row r="21">
       <c r="A21" s="51" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B21" s="51" t="s">
         <v>164</v>
@@ -8841,7 +8841,7 @@
         <v>150</v>
       </c>
       <c r="I21" s="59" t="s">
-        <v>214</v>
+        <v>185</v>
       </c>
       <c r="J21" s="54" t="s">
         <v>189</v>
@@ -8874,7 +8874,7 @@
         <v>197</v>
       </c>
       <c r="I22" s="59" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J22" s="54" t="s">
         <v>139</v>
@@ -8883,7 +8883,7 @@
         <v>200</v>
       </c>
       <c r="L22" s="59" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="M22" s="63"/>
       <c r="N22" s="63"/>
@@ -8914,8 +8914,8 @@
       <c r="B24" s="51" t="s">
         <v>147</v>
       </c>
-      <c r="C24" s="62" t="s">
-        <v>226</v>
+      <c r="C24" s="70" t="s">
+        <v>225</v>
       </c>
       <c r="D24" s="68"/>
       <c r="E24" s="68"/>
@@ -8929,8 +8929,8 @@
       <c r="B25" s="51" t="s">
         <v>147</v>
       </c>
-      <c r="C25" s="62" t="s">
-        <v>227</v>
+      <c r="C25" s="70" t="s">
+        <v>226</v>
       </c>
       <c r="D25" s="68"/>
       <c r="E25" s="68"/>
@@ -8944,8 +8944,8 @@
       <c r="B26" s="51" t="s">
         <v>147</v>
       </c>
-      <c r="C26" s="62" t="s">
-        <v>227</v>
+      <c r="C26" s="70" t="s">
+        <v>226</v>
       </c>
       <c r="D26" s="68"/>
       <c r="E26" s="68"/>
@@ -8959,8 +8959,8 @@
       <c r="B27" s="51" t="s">
         <v>147</v>
       </c>
-      <c r="C27" s="62" t="s">
-        <v>227</v>
+      <c r="C27" s="70" t="s">
+        <v>226</v>
       </c>
       <c r="D27" s="68"/>
       <c r="E27" s="68"/>
@@ -8974,8 +8974,8 @@
       <c r="B28" s="51" t="s">
         <v>147</v>
       </c>
-      <c r="C28" s="62" t="s">
-        <v>227</v>
+      <c r="C28" s="70" t="s">
+        <v>226</v>
       </c>
       <c r="D28" s="68"/>
       <c r="E28" s="68"/>
@@ -8989,8 +8989,8 @@
       <c r="B29" s="51" t="s">
         <v>147</v>
       </c>
-      <c r="C29" s="62" t="s">
-        <v>227</v>
+      <c r="C29" s="70" t="s">
+        <v>226</v>
       </c>
       <c r="D29" s="68"/>
       <c r="E29" s="68"/>
@@ -9004,8 +9004,8 @@
       <c r="B30" s="51" t="s">
         <v>179</v>
       </c>
-      <c r="C30" s="62" t="s">
-        <v>228</v>
+      <c r="C30" s="70" t="s">
+        <v>227</v>
       </c>
       <c r="D30" s="68"/>
       <c r="E30" s="68"/>
@@ -9019,8 +9019,8 @@
       <c r="B31" s="51" t="s">
         <v>202</v>
       </c>
-      <c r="C31" s="62" t="s">
-        <v>228</v>
+      <c r="C31" s="70" t="s">
+        <v>227</v>
       </c>
       <c r="D31" s="68"/>
       <c r="E31" s="68"/>
@@ -9034,8 +9034,8 @@
       <c r="B32" s="51" t="s">
         <v>206</v>
       </c>
-      <c r="C32" s="62" t="s">
-        <v>228</v>
+      <c r="C32" s="70" t="s">
+        <v>227</v>
       </c>
       <c r="D32" s="68"/>
       <c r="E32" s="68"/>
@@ -9049,8 +9049,8 @@
       <c r="B33" s="51" t="s">
         <v>210</v>
       </c>
-      <c r="C33" s="62" t="s">
-        <v>228</v>
+      <c r="C33" s="70" t="s">
+        <v>227</v>
       </c>
       <c r="D33" s="68"/>
       <c r="E33" s="68"/>
@@ -9062,10 +9062,10 @@
         <v>134</v>
       </c>
       <c r="B34" s="51" t="s">
-        <v>215</v>
-      </c>
-      <c r="C34" s="62" t="s">
-        <v>228</v>
+        <v>214</v>
+      </c>
+      <c r="C34" s="70" t="s">
+        <v>227</v>
       </c>
       <c r="D34" s="68"/>
       <c r="E34" s="68"/>
@@ -9077,10 +9077,10 @@
         <v>134</v>
       </c>
       <c r="B35" s="51" t="s">
-        <v>219</v>
-      </c>
-      <c r="C35" s="62" t="s">
-        <v>228</v>
+        <v>218</v>
+      </c>
+      <c r="C35" s="70" t="s">
+        <v>227</v>
       </c>
       <c r="D35" s="68"/>
       <c r="E35" s="68"/>
@@ -9092,10 +9092,10 @@
         <v>134</v>
       </c>
       <c r="B36" s="51" t="s">
-        <v>223</v>
-      </c>
-      <c r="C36" s="62" t="s">
-        <v>228</v>
+        <v>222</v>
+      </c>
+      <c r="C36" s="70" t="s">
+        <v>227</v>
       </c>
       <c r="D36" s="68"/>
       <c r="E36" s="68"/>
@@ -9189,19 +9189,19 @@
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2">
@@ -9215,19 +9215,19 @@
         <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>28</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3">
@@ -9241,19 +9241,19 @@
         <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>25</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>29</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="4">
@@ -9267,19 +9267,19 @@
         <v>16</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5">
@@ -9287,19 +9287,19 @@
         <v>17</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>23</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6">
@@ -9307,19 +9307,19 @@
         <v>18</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>27</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>33</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7">
@@ -9327,19 +9327,19 @@
         <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>248</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>249</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>31</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8">
@@ -9347,7 +9347,7 @@
         <v>32</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -9401,7 +9401,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2">
@@ -9409,7 +9409,7 @@
         <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3">
@@ -9417,7 +9417,7 @@
         <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4">
@@ -9425,7 +9425,7 @@
         <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5">
@@ -9433,7 +9433,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="6">
@@ -9441,7 +9441,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7">
@@ -9449,7 +9449,7 @@
         <v>19</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8">
@@ -10466,7 +10466,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2">
@@ -10474,7 +10474,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3">
@@ -10482,7 +10482,7 @@
         <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4">
@@ -10490,7 +10490,7 @@
         <v>26</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5">
@@ -10498,7 +10498,7 @@
         <v>22</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="6">
@@ -10506,15 +10506,15 @@
         <v>27</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>248</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="8">
@@ -11536,7 +11536,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2">
@@ -11544,7 +11544,7 @@
         <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3">
@@ -11552,7 +11552,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="4">
@@ -11560,7 +11560,7 @@
         <v>30</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5">
@@ -11568,7 +11568,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6">
@@ -11576,7 +11576,7 @@
         <v>33</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7">
@@ -11584,7 +11584,7 @@
         <v>31</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8">
@@ -11592,7 +11592,7 @@
         <v>32</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="9">

</xml_diff>